<commit_message>
fix state level date duplication
</commit_message>
<xml_diff>
--- a/original-sources/historical/hhs/hhs_data_2020-07-30.xlsx
+++ b/original-sources/historical/hhs/hhs_data_2020-07-30.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">ï..OBJECTID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">Shape__Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Alaska</t>
@@ -403,13 +406,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -432,8 +440,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,19 +767,22 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
@@ -789,6 +801,9 @@
       </c>
       <c r="J2" t="n">
         <v>407.570958324101</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="3">
@@ -796,13 +811,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="n">
         <v>9</v>
@@ -821,6 +836,9 @@
       </c>
       <c r="J3" t="n">
         <v>42.2601574991052</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="4">
@@ -828,13 +846,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
         <v>9</v>
@@ -853,6 +871,9 @@
       </c>
       <c r="J4" t="n">
         <v>11.9527869436732</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="5">
@@ -860,13 +881,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
@@ -885,6 +906,9 @@
       </c>
       <c r="J5" t="n">
         <v>28.5296728484553</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="6">
@@ -892,13 +916,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="n">
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n">
         <v>9</v>
@@ -917,6 +941,9 @@
       </c>
       <c r="J6" t="n">
         <v>23.6087337781305</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="7">
@@ -924,13 +951,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="n">
         <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" t="n">
         <v>10</v>
@@ -949,6 +976,9 @@
       </c>
       <c r="J7" t="n">
         <v>24.7872488348153</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="8">
@@ -956,13 +986,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="n">
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
@@ -981,6 +1011,9 @@
       </c>
       <c r="J8" t="n">
         <v>34.9568573750297</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="9">
@@ -988,13 +1021,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="n">
         <v>9</v>
@@ -1013,6 +1046,9 @@
       </c>
       <c r="J9" t="n">
         <v>23.2572697290375</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="10">
@@ -1020,13 +1056,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="n">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="n">
         <v>6</v>
@@ -1045,6 +1081,9 @@
       </c>
       <c r="J10" t="n">
         <v>20.877179341548</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="11">
@@ -1052,13 +1091,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="n">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="n">
         <v>8</v>
@@ -1077,6 +1116,9 @@
       </c>
       <c r="J11" t="n">
         <v>22.0256262721942</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="12">
@@ -1084,13 +1126,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="n">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" t="n">
         <v>7</v>
@@ -1109,6 +1151,9 @@
       </c>
       <c r="J12" t="n">
         <v>18.7903206413307</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="13">
@@ -1116,13 +1161,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="n">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" t="n">
         <v>7</v>
@@ -1141,6 +1186,9 @@
       </c>
       <c r="J13" t="n">
         <v>21.1048705539639</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="14">
@@ -1148,13 +1196,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" t="n">
         <v>6</v>
@@ -1173,6 +1221,9 @@
       </c>
       <c r="J14" t="n">
         <v>32.5702758640733</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="15">
@@ -1180,13 +1231,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="n">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" t="n">
         <v>5</v>
@@ -1205,6 +1256,9 @@
       </c>
       <c r="J15" t="n">
         <v>29.5110548878106</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="16">
@@ -1212,13 +1266,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="n">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" t="n">
         <v>7</v>
@@ -1237,6 +1291,9 @@
       </c>
       <c r="J16" t="n">
         <v>23.5959465236339</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="17">
@@ -1244,13 +1301,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="n">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" t="n">
         <v>8</v>
@@ -1269,6 +1326,9 @@
       </c>
       <c r="J17" t="n">
         <v>34.5280658083754</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="18">
@@ -1276,13 +1336,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" t="n">
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" t="n">
         <v>7</v>
@@ -1301,6 +1361,9 @@
       </c>
       <c r="J18" t="n">
         <v>23.3833196259553</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="19">
@@ -1308,13 +1371,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" t="n">
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" t="n">
         <v>6</v>
@@ -1333,6 +1396,9 @@
       </c>
       <c r="J19" t="n">
         <v>23.5377110630426</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="20">
@@ -1340,13 +1406,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="n">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" t="n">
         <v>8</v>
@@ -1365,6 +1431,9 @@
       </c>
       <c r="J20" t="n">
         <v>21.3533067056279</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="21">
@@ -1372,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="n">
         <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" t="n">
         <v>6</v>
@@ -1397,6 +1466,9 @@
       </c>
       <c r="J21" t="n">
         <v>25.5572653890967</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="22">
@@ -1404,13 +1476,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="n">
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" t="n">
         <v>8</v>
@@ -1429,6 +1501,9 @@
       </c>
       <c r="J22" t="n">
         <v>22.746545647107</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="23">
@@ -1436,13 +1511,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="n">
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E23" t="n">
         <v>6</v>
@@ -1461,6 +1536,9 @@
       </c>
       <c r="J23" t="n">
         <v>64.8074583859905</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="24">
@@ -1468,13 +1546,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" t="n">
         <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E24" t="n">
         <v>8</v>
@@ -1493,6 +1571,9 @@
       </c>
       <c r="J24" t="n">
         <v>19.9922227331591</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="25">
@@ -1500,13 +1581,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="n">
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" t="n">
         <v>8</v>
@@ -1525,6 +1606,9 @@
       </c>
       <c r="J25" t="n">
         <v>21.9870299734703</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="26">
@@ -1532,13 +1616,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E26" t="n">
         <v>4</v>
@@ -1557,6 +1641,9 @@
       </c>
       <c r="J26" t="n">
         <v>17.2376579292563</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="27">
@@ -1564,13 +1651,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" t="n">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1589,6 +1676,9 @@
       </c>
       <c r="J27" t="n">
         <v>5.72245921907398</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="28">
@@ -1596,13 +1686,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="n">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E28" t="n">
         <v>3</v>
@@ -1621,6 +1711,9 @@
       </c>
       <c r="J28" t="n">
         <v>4.07536505514256</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="29">
@@ -1628,13 +1721,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" t="n">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
@@ -1653,6 +1746,9 @@
       </c>
       <c r="J29" t="n">
         <v>0.632462402279614</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="30">
@@ -1660,13 +1756,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30" t="n">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E30" t="n">
         <v>4</v>
@@ -1685,6 +1781,9 @@
       </c>
       <c r="J30" t="n">
         <v>41.0850101590848</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="31">
@@ -1692,13 +1791,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31" t="n">
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E31" t="n">
         <v>4</v>
@@ -1717,6 +1816,9 @@
       </c>
       <c r="J31" t="n">
         <v>20.1034674931405</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="32">
@@ -1724,13 +1826,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" t="n">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E32" t="n">
         <v>5</v>
@@ -1749,6 +1851,9 @@
       </c>
       <c r="J32" t="n">
         <v>19.9992245695128</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="33">
@@ -1756,13 +1861,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" t="n">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E33" t="n">
         <v>5</v>
@@ -1781,6 +1886,9 @@
       </c>
       <c r="J33" t="n">
         <v>16.1103069470809</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="34">
@@ -1788,13 +1896,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" t="n">
         <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E34" t="n">
         <v>4</v>
@@ -1813,6 +1921,9 @@
       </c>
       <c r="J34" t="n">
         <v>21.1523487327623</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="35">
@@ -1820,13 +1931,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" t="n">
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
@@ -1845,6 +1956,9 @@
       </c>
       <c r="J35" t="n">
         <v>18.8987201269951</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="36">
@@ -1852,13 +1966,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C36" t="n">
         <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E36" t="n">
         <v>3</v>
@@ -1877,6 +1991,9 @@
       </c>
       <c r="J36" t="n">
         <v>21.8809236006354</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="37">
@@ -1884,13 +2001,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" t="n">
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E37" t="n">
         <v>1</v>
@@ -1909,6 +2026,9 @@
       </c>
       <c r="J37" t="n">
         <v>13.1051255991428</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="38">
@@ -1916,13 +2036,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C38" t="n">
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E38" t="n">
         <v>5</v>
@@ -1941,6 +2061,9 @@
       </c>
       <c r="J38" t="n">
         <v>40.8232803907847</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="39">
@@ -1948,13 +2071,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C39" t="n">
         <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E39" t="n">
         <v>4</v>
@@ -1973,6 +2096,9 @@
       </c>
       <c r="J39" t="n">
         <v>22.0600157416285</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="40">
@@ -1980,13 +2106,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C40" t="n">
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
@@ -2005,6 +2131,9 @@
       </c>
       <c r="J40" t="n">
         <v>8.37458017541608</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="41">
@@ -2012,13 +2141,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C41" t="n">
         <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E41" t="n">
         <v>2</v>
@@ -2037,6 +2166,9 @@
       </c>
       <c r="J41" t="n">
         <v>8.41959364715719</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="42">
@@ -2044,13 +2176,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C42" t="n">
         <v>36</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E42" t="n">
         <v>2</v>
@@ -2069,6 +2201,9 @@
       </c>
       <c r="J42" t="n">
         <v>28.4874693243922</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="43">
@@ -2076,13 +2211,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C43" t="n">
         <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E43" t="n">
         <v>4</v>
@@ -2101,6 +2236,9 @@
       </c>
       <c r="J43" t="n">
         <v>34.5834965407093</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="44">
@@ -2108,13 +2246,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" t="n">
         <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E44" t="n">
         <v>5</v>
@@ -2133,6 +2271,9 @@
       </c>
       <c r="J44" t="n">
         <v>16.1304354133078</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="45">
@@ -2140,13 +2281,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" t="n">
         <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E45" t="n">
         <v>3</v>
@@ -2165,6 +2306,9 @@
       </c>
       <c r="J45" t="n">
         <v>16.8410838362311</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="46">
@@ -2172,13 +2316,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C46" t="n">
         <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
@@ -2197,6 +2341,9 @@
       </c>
       <c r="J46" t="n">
         <v>3.64267357764134</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="47">
@@ -2204,13 +2351,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C47" t="n">
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E47" t="n">
         <v>4</v>
@@ -2229,6 +2376,9 @@
       </c>
       <c r="J47" t="n">
         <v>16.1270830720728</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="48">
@@ -2236,13 +2386,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" t="n">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E48" t="n">
         <v>4</v>
@@ -2261,6 +2411,9 @@
       </c>
       <c r="J48" t="n">
         <v>21.4603363220314</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="49">
@@ -2268,13 +2421,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49" t="n">
         <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E49" t="n">
         <v>1</v>
@@ -2293,6 +2446,9 @@
       </c>
       <c r="J49" t="n">
         <v>8.45014587394864</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="50">
@@ -2300,13 +2456,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" t="n">
         <v>51</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
@@ -2325,6 +2481,9 @@
       </c>
       <c r="J50" t="n">
         <v>31.1995914738484</v>
+      </c>
+      <c r="K50" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="51">
@@ -2332,13 +2491,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" t="n">
         <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E51" t="n">
         <v>3</v>
@@ -2357,6 +2516,9 @@
       </c>
       <c r="J51" t="n">
         <v>18.1962363076172</v>
+      </c>
+      <c r="K51" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="52">
@@ -2364,13 +2526,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C52" t="n">
         <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E52" t="n">
         <v>5</v>
@@ -2389,6 +2551,9 @@
       </c>
       <c r="J52" t="n">
         <v>21.8914009902698</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="53">
@@ -2396,13 +2561,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C53" t="n">
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E53" t="n">
         <v>9</v>
@@ -2421,6 +2586,9 @@
       </c>
       <c r="J53" t="n">
         <v>0.600124356952566</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="54">
@@ -2428,13 +2596,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C54" t="n">
         <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E54" t="n">
         <v>9</v>
@@ -2453,6 +2621,9 @@
       </c>
       <c r="J54" t="n">
         <v>1.12001626312496</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="55">
@@ -2460,13 +2631,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" t="n">
         <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E55" t="n">
         <v>9</v>
@@ -2485,6 +2656,9 @@
       </c>
       <c r="J55" t="n">
         <v>0.683479015444908</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="56">
@@ -2492,13 +2666,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C56" t="n">
         <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E56" t="n">
         <v>9</v>
@@ -2517,6 +2691,9 @@
       </c>
       <c r="J56" t="n">
         <v>0.908853027385353</v>
+      </c>
+      <c r="K56" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="57">
@@ -2524,13 +2701,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C57" t="n">
         <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E57" t="n">
         <v>2</v>
@@ -2549,6 +2726,9 @@
       </c>
       <c r="J57" t="n">
         <v>4.78861765850568</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="58">
@@ -2556,13 +2736,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" t="n">
         <v>78</v>
       </c>
       <c r="D58" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E58" t="n">
         <v>2</v>
@@ -2581,6 +2761,9 @@
       </c>
       <c r="J58" t="n">
         <v>1.23662789403411</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
     <row r="59">
@@ -2588,13 +2771,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C59" t="n">
         <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E59" t="n">
         <v>9</v>
@@ -2608,19 +2791,22 @@
       <c r="J59" t="n">
         <v>1.1053233016917</v>
       </c>
+      <c r="K59" s="1" t="n">
+        <v>44042</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C60" t="n">
         <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E60" t="n">
         <v>9</v>
@@ -2639,6 +2825,9 @@
       </c>
       <c r="J60" t="n">
         <v>1.04242124055477</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>44042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>